<commit_message>
Add file for tests, and script for them
</commit_message>
<xml_diff>
--- a/Data/TabStats_Short.xlsx
+++ b/Data/TabStats_Short.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A14B5D9-839D-4E89-B2F3-A23D25E300FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5DF669-8A93-4A80-8705-DBF0CB327DD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="36">
   <si>
     <t>DATES</t>
   </si>
@@ -59,6 +59,75 @@
   </si>
   <si>
     <t>Alex</t>
+  </si>
+  <si>
+    <t>Luc</t>
+  </si>
+  <si>
+    <t>Flora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flora </t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Lucie</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Lydie</t>
+  </si>
+  <si>
+    <t>Rémi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Céline </t>
+  </si>
+  <si>
+    <t>Davy</t>
+  </si>
+  <si>
+    <t>Alain</t>
+  </si>
+  <si>
+    <t>Thibaud</t>
+  </si>
+  <si>
+    <t>Céline</t>
+  </si>
+  <si>
+    <t>Celine</t>
+  </si>
+  <si>
+    <t>René</t>
+  </si>
+  <si>
+    <t>Alix</t>
+  </si>
+  <si>
+    <t>Louise</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Elise</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Solen</t>
   </si>
 </sst>
 </file>
@@ -106,7 +175,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="33">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -160,20 +289,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6EA7BF90-13D7-44A2-86DC-CD53BAD3819B}" name="Tableau1" displayName="Tableau1" ref="A1:K63" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K63" xr:uid="{5EA3D26D-38A6-4BF3-B601-454D2F09D8A6}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B4F8A008-CA82-45B5-937C-82CB5F6E68AC}" name="DATES" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{67881ED4-59FC-4187-B21E-18AC83770A82}" name="Paul" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{F28B1D1A-CE77-404B-BC4D-116958A1E710}" name="Lise" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{D591B1A1-3481-4F9F-B1AF-8D3E03EA174D}" name="Pierre" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{34E9D56D-A7CB-4F57-99F7-F445188C4AA4}" name="Marie" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{40D78A82-472D-44B4-A68F-41E306804347}" name=" Eric" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{857D41DE-C2AD-4DB5-BBA5-A873F8E7DE42}" name="Manon" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{12111A7C-BEE4-4D8F-8784-A4E4F63073D2}" name=" Alex" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{F26000AE-7FCF-459E-8C35-52B19539C5CE}" name="Sarah" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{846E6367-2762-4049-A58D-F99E23870A53}" name="David" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{298EB763-EDAB-47E0-BE2B-24F35C489C0D}" name="Inès" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6EA7BF90-13D7-44A2-86DC-CD53BAD3819B}" name="Tableau1" displayName="Tableau1" ref="A1:AE63" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:AE63" xr:uid="{5EA3D26D-38A6-4BF3-B601-454D2F09D8A6}"/>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{B4F8A008-CA82-45B5-937C-82CB5F6E68AC}" name="DATES" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{67881ED4-59FC-4187-B21E-18AC83770A82}" name="Paul" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{F28B1D1A-CE77-404B-BC4D-116958A1E710}" name="Lise" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{D591B1A1-3481-4F9F-B1AF-8D3E03EA174D}" name="Pierre" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{34E9D56D-A7CB-4F57-99F7-F445188C4AA4}" name="Marie" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{40D78A82-472D-44B4-A68F-41E306804347}" name=" Eric" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{857D41DE-C2AD-4DB5-BBA5-A873F8E7DE42}" name="Manon" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{12111A7C-BEE4-4D8F-8784-A4E4F63073D2}" name=" Alex" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{F26000AE-7FCF-459E-8C35-52B19539C5CE}" name="Sarah" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{846E6367-2762-4049-A58D-F99E23870A53}" name="David" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{298EB763-EDAB-47E0-BE2B-24F35C489C0D}" name="Inès" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{CF291B7F-78CE-46E0-8EDE-8A878F4E0C07}" name="Luc" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{F9FD7236-EC9A-4222-9E26-0B9B48366024}" name="Flora" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{C9D2DA9A-C1A2-4E0A-8FB5-1CE7EBA52F8C}" name="Louis" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{F17C7706-2E5B-4A6F-AACD-0808D472EBCC}" name="Lucie" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{DF7E1FF4-E538-4DA8-94CC-6FE81CEA0678}" name="Jean" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{334AE403-3B57-40AA-B358-58342762DFF2}" name="Sophie" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{D5A35165-0339-416D-84B4-352562C6D811}" name="Patrick" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{9F75A2C7-20DB-4241-8B5C-959687F44016}" name="Lydie" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{D0C3954F-83A2-416F-B12F-AAD67B3EACED}" name="Rémi" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{6EEDAB00-43CF-428B-8CDC-3C4175D71DD5}" name="Celine" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{26E3E1C3-A7BF-4494-B4BF-BB6A65108FBE}" name="Davy" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{A8462C46-E977-4B0C-8C92-AEC0639E80F8}" name="Alain" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{A3FA12A8-A316-41C4-985F-9046DDA6CB1E}" name="Thibaud" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{1BF201FB-FA3D-4630-92E2-6C8B7FD53A23}" name="René" dataDxfId="6"/>
+    <tableColumn id="26" xr3:uid="{CDE91431-2AA7-43BD-AA6B-25EFCAD3B1F4}" name="Alix" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{92FA058B-55DF-49B8-A1F5-EBF7417ABA10}" name="Louise" dataDxfId="4"/>
+    <tableColumn id="28" xr3:uid="{191E1D86-6166-448B-ACB7-C9F75043CD02}" name="Lucas" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{FE0AADB5-2585-45FD-8D5D-2C8AE8F205D7}" name="Elise" dataDxfId="2"/>
+    <tableColumn id="30" xr3:uid="{98154592-DA44-4C84-98A1-7647F91F6242}" name="Sandra" dataDxfId="1"/>
+    <tableColumn id="31" xr3:uid="{BEC86A20-1CF6-47D2-B077-2E4DE50C2B62}" name="Solen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -442,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:AE63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +607,7 @@
     <col min="65" max="65" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,8 +641,68 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43101</v>
       </c>
@@ -521,8 +730,52 @@
       <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -544,8 +797,46 @@
       <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43102</v>
       </c>
@@ -573,8 +864,46 @@
         <v>9</v>
       </c>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -596,8 +925,48 @@
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE5" s="1"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43103</v>
       </c>
@@ -621,8 +990,48 @@
         <v>9</v>
       </c>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -644,8 +1053,52 @@
       <c r="K7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE7" s="1"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43104</v>
       </c>
@@ -669,8 +1122,44 @@
       <c r="K8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -688,8 +1177,38 @@
         <v>9</v>
       </c>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43105</v>
       </c>
@@ -715,8 +1234,50 @@
       <c r="K10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE10" s="1"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -734,8 +1295,50 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43106</v>
       </c>
@@ -761,8 +1364,48 @@
         <v>9</v>
       </c>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE12" s="1"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -782,8 +1425,46 @@
       <c r="K13" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43107</v>
       </c>
@@ -807,8 +1488,48 @@
       <c r="K14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
@@ -826,8 +1547,48 @@
         <v>9</v>
       </c>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE15" s="1"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43108</v>
       </c>
@@ -855,8 +1616,50 @@
       <c r="K16" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -878,8 +1681,50 @@
       <c r="K17" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE17" s="1"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43109</v>
       </c>
@@ -907,8 +1752,46 @@
         <v>9</v>
       </c>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE18" s="1"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>1</v>
@@ -930,8 +1813,52 @@
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43110</v>
       </c>
@@ -955,8 +1882,46 @@
         <v>9</v>
       </c>
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
@@ -978,8 +1943,54 @@
       <c r="K21" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43111</v>
       </c>
@@ -1007,8 +2018,50 @@
       <c r="K22" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
@@ -1030,8 +2083,46 @@
       <c r="K23" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="1"/>
+      <c r="M23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE23" s="1"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43112</v>
       </c>
@@ -1059,8 +2150,48 @@
         <v>9</v>
       </c>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>1</v>
@@ -1082,8 +2213,48 @@
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43113</v>
       </c>
@@ -1107,8 +2278,48 @@
         <v>9</v>
       </c>
       <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
@@ -1130,8 +2341,50 @@
       <c r="K27" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="1"/>
+      <c r="M27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE27" s="1"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43114</v>
       </c>
@@ -1155,8 +2408,44 @@
       <c r="K28" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
@@ -1174,8 +2463,40 @@
         <v>9</v>
       </c>
       <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43115</v>
       </c>
@@ -1201,8 +2522,50 @@
       <c r="K30" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE30" s="1"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
@@ -1220,8 +2583,50 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43116</v>
       </c>
@@ -1247,8 +2652,46 @@
         <v>9</v>
       </c>
       <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE32" s="1"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
@@ -1268,8 +2711,46 @@
       <c r="K33" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43117</v>
       </c>
@@ -1293,8 +2774,44 @@
       <c r="K34" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
@@ -1312,8 +2829,50 @@
         <v>9</v>
       </c>
       <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43118</v>
       </c>
@@ -1341,8 +2900,48 @@
       <c r="K36" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
@@ -1364,8 +2963,50 @@
       <c r="K37" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="1"/>
+      <c r="M37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43119</v>
       </c>
@@ -1393,8 +3034,44 @@
         <v>9</v>
       </c>
       <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>1</v>
@@ -1416,8 +3093,50 @@
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE39" s="1"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43120</v>
       </c>
@@ -1441,8 +3160,50 @@
         <v>9</v>
       </c>
       <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
@@ -1464,8 +3225,50 @@
       <c r="K41" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE41" s="1"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43121</v>
       </c>
@@ -1493,8 +3296,48 @@
         <v>9</v>
       </c>
       <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE42" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>1</v>
@@ -1516,8 +3359,50 @@
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD43" s="1"/>
+      <c r="AE43" s="1"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43122</v>
       </c>
@@ -1545,8 +3430,48 @@
       <c r="K44" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD44" s="1"/>
+      <c r="AE44" s="1"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
@@ -1568,8 +3493,52 @@
       <c r="K45" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="1"/>
+      <c r="M45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43123</v>
       </c>
@@ -1595,8 +3564,44 @@
       <c r="K46" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE46" s="1"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
@@ -1618,8 +3623,46 @@
         <v>9</v>
       </c>
       <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="1"/>
+      <c r="M47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43124</v>
       </c>
@@ -1643,8 +3686,46 @@
         <v>9</v>
       </c>
       <c r="K48" s="1"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD48" s="1"/>
+      <c r="AE48" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
@@ -1666,8 +3747,46 @@
       <c r="K49" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE49" s="1"/>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43125</v>
       </c>
@@ -1693,8 +3812,44 @@
       <c r="K50" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
@@ -1714,8 +3869,50 @@
         <v>9</v>
       </c>
       <c r="K51" s="1"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB51" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC51" s="1"/>
+      <c r="AD51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE51" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43126</v>
       </c>
@@ -1741,8 +3938,46 @@
       <c r="K52" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC52" s="1"/>
+      <c r="AD52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE52" s="1"/>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
@@ -1760,8 +3995,52 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD53" s="1"/>
+      <c r="AE53" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43127</v>
       </c>
@@ -1787,8 +4066,46 @@
         <v>9</v>
       </c>
       <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB54" s="1"/>
+      <c r="AC54" s="1"/>
+      <c r="AD54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE54" s="1"/>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
@@ -1808,8 +4125,46 @@
       <c r="K55" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="1"/>
+      <c r="M55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA55" s="1"/>
+      <c r="AB55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD55" s="1"/>
+      <c r="AE55" s="1"/>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43128</v>
       </c>
@@ -1833,8 +4188,46 @@
       <c r="K56" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE56" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
@@ -1852,8 +4245,42 @@
         <v>9</v>
       </c>
       <c r="K57" s="1"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="1"/>
+      <c r="M57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC57" s="1"/>
+      <c r="AD57" s="1"/>
+      <c r="AE57" s="1"/>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43129</v>
       </c>
@@ -1881,8 +4308,48 @@
       <c r="K58" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
+      <c r="AC58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD58" s="1"/>
+      <c r="AE58" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
@@ -1904,8 +4371,48 @@
       <c r="K59" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="1"/>
+      <c r="M59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+      <c r="AD59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE59" s="1"/>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43130</v>
       </c>
@@ -1931,8 +4438,50 @@
       <c r="K60" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC60" s="1"/>
+      <c r="AD60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE60" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
         <v>1</v>
@@ -1956,8 +4505,50 @@
       <c r="K61" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="1"/>
+      <c r="M61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD61" s="1"/>
+      <c r="AE61" s="1"/>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>43131</v>
       </c>
@@ -1983,8 +4574,44 @@
       <c r="K62" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z62" s="1"/>
+      <c r="AA62" s="1"/>
+      <c r="AB62" s="1"/>
+      <c r="AC62" s="1"/>
+      <c r="AD62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE62" s="1"/>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
@@ -2006,6 +4633,44 @@
         <v>9</v>
       </c>
       <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+      <c r="AA63" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD63" s="1"/>
+      <c r="AE63" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>